<commit_message>
Merge of ESPNow with Bluetooth and fx1901 Sensor
Left_Slave reads values from fx1901 and sends them to Right_Master for further processing. Right_Master transmits both values via bluetooth

calibration excel has been updated
</commit_message>
<xml_diff>
--- a/Backend/Fx1901_Test/calibration.xlsx
+++ b/Backend/Fx1901_Test/calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a223857592d5ea4/HS-Karlsruhe/Microcontroller (Walter)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="8_{5202EC2A-2471-44AF-9DB1-3722DF246BDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CD84AB0A-FBB6-432E-8594-CB6FF4050219}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="8_{5202EC2A-2471-44AF-9DB1-3722DF246BDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{02E38EFA-5989-409A-9E02-4AC23C41E648}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14C2035C-873D-49F6-AB31-095275858BAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{14C2035C-873D-49F6-AB31-095275858BAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Kalibrierung iUAGS1" sheetId="2" r:id="rId1"/>
@@ -560,6 +560,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Raw sensor data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1188,6 +1213,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>korrigierten</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" baseline="0"/>
+              <a:t> Werte</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1226,6 +1281,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>iUAGS</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1306,10 +1364,55 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Kalibrierung iUAGS2'!$E$3:$E$17</c:f>
+              <c:f>'Kalibrierung iUAGS2'!$D$3:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-9006.9050077439333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1359.7702632937526</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7352.1553949406307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16064.081053175014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25098.670624677336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33165.268456375838</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37359.899328859057</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39295.882808466704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44458.50542075374</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47039.816726897261</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49943.791946308724</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52202.439339184304</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56397.070211667524</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59301.045431078986</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67690.307176045419</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1317,6 +1420,151 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3098-4698-A00A-338D147BE722}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>iUAGS2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Kalibrierung iUAGS1'!$A$3:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Kalibrierung iUAGS1'!$D$3:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-10740.136726793509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2709.496746561239</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7998.0232270817896</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18705.543200724816</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26118.441644016148</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29824.890865661811</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37649.617000247097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42179.721604480685</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44650.687752244456</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46709.826208714272</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50004.447739065974</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>53299.069269417676</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56181.863108475409</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59064.656947533156</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66065.727699530515</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-112E-4C72-A620-70ADB06CC4F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3172,16 +3420,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>438149</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>123824</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3216,15 +3464,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>161924</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>695324</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3253,14 +3501,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>61912</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3587,8 +3835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F02671-C0B0-4C9D-968C-D213B77272A4}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3630,7 +3878,7 @@
       </c>
       <c r="D3">
         <f>B3/$C$22-$C$21/$C$22</f>
-        <v>-9265.0361383582858</v>
+        <v>-10740.136726793509</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3642,7 +3890,7 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D17" si="0">B4/$C$22-$C$21/$C$22</f>
-        <v>-2973.0898296334535</v>
+        <v>-2709.496746561239</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3654,7 +3902,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>5416.1719153329896</v>
+        <v>7998.0232270817896</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3666,7 +3914,7 @@
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>13805.433660299434</v>
+        <v>18705.543200724816</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3678,7 +3926,7 @@
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>19613.384099122355</v>
+        <v>26118.441644016148</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3690,7 +3938,7 @@
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>22517.359318533814</v>
+        <v>29824.890865661811</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3702,7 +3950,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>28647.973670624677</v>
+        <v>37649.617000247097</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3714,7 +3962,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>32197.276716572022</v>
+        <v>42179.721604480685</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3726,7 +3974,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>34133.260196179661</v>
+        <v>44650.687752244456</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3738,7 +3986,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>35746.579762519359</v>
+        <v>46709.826208714272</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3750,7 +3998,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>38327.891068662881</v>
+        <v>50004.447739065974</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3762,7 +4010,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>40909.202374806402</v>
+        <v>53299.069269417676</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3774,7 +4022,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>43167.849767681982</v>
+        <v>56181.863108475409</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3786,7 +4034,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>45426.497160557563</v>
+        <v>59064.656947533156</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3798,7 +4046,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>50911.783686112547</v>
+        <v>66065.727699530515</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3809,7 +4057,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>202142</v>
+        <v>175792</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3817,7 +4065,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>30.992000000000001</v>
+        <v>24.282</v>
       </c>
     </row>
   </sheetData>
@@ -3830,14 +4078,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D840CEEC-5F72-44DA-86BE-17F0F5C56247}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>